<commit_message>
scraped universities from A to Muş
</commit_message>
<xml_diff>
--- a/data/universities.xlsx
+++ b/data/universities.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,18 +433,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ACIBADEM MEHMET ALİ AYDINLAR ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://akademik.yok.gov.tr/AkademikArama/AkademisyenArama?islem=2qW3CPZt7b-w2_C8bs95zcm3PLoRf9yvy9mnk3CteLrv96FgaKCkCWcpWlro_ywH</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>